<commit_message>
Added excel sheets and graph pictures
</commit_message>
<xml_diff>
--- a/load_test/t2_micro.xlsx
+++ b/load_test/t2_micro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Computerzor\Desktop\Dinnerpal\dinner-pal\load_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D640B1-B0BA-4F16-BE6B-565C4F1FECEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4628B22-BF51-416F-BCF2-E665F05154B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{470D2FEA-53B5-445C-B75C-2F219D3B4E02}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
     <t>time</t>
   </si>
@@ -419,6 +419,7 @@
         <c:axId val="408191576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="350"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2071,6 +2072,7 @@
         <c:axId val="408191576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="350"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3877,9 +3879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40CED862-F276-434A-A0AA-467A8A9FBBFD}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -4133,9 +4133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645985D4-FE42-4A47-85CA-41458B4BAC19}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>

</xml_diff>